<commit_message>
created yielder for costs and premiums
</commit_message>
<xml_diff>
--- a/Tablas.xlsx
+++ b/Tablas.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC490FF-F383-4DCC-897D-C877F7F33C7F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B89AB4F-710D-428D-8316-913E776E87F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inicial_H" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
   <si>
     <t>100+</t>
   </si>
@@ -391,8 +391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B3BDBC-AAC9-49B1-855A-0D97D040112E}">
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,8 +499,8 @@
       <c r="AE1" s="1">
         <v>29</v>
       </c>
-      <c r="AF1" s="1">
-        <v>30</v>
+      <c r="AF1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
@@ -511,25 +511,25 @@
         <v>13218</v>
       </c>
       <c r="C2">
-        <v>26437</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>46264</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>26437</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>13218</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>3965</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1322</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1322</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -612,22 +612,22 @@
         <v>30435</v>
       </c>
       <c r="D3">
-        <v>53261</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>30435</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>15217</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>4565</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>1522</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1522</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -713,19 +713,19 @@
         <v>53264</v>
       </c>
       <c r="E4">
-        <v>30437</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>15218</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>4566</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1522</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1522</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -10410,8 +10410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3891B7-828C-4C9D-A5A3-A41D0B8931D1}">
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="K108" sqref="K108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20426,8 +20426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB30A8E-EAFD-4DB6-A194-D6447164BAE7}">
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21261,7 +21261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265E6485-F743-4A15-8A53-86D09FBD23C8}">
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -22096,8 +22096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558351FC-9FCA-4CDD-A3D5-63FE9C2CB36B}">
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="Q85" sqref="Q85"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32111,8 +32111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8480506-65EC-4396-9F63-D6C89905E883}">
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>